<commit_message>
Add Change Language Button
</commit_message>
<xml_diff>
--- a/languages.xlsx
+++ b/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E966BA8C-70C1-4CB0-ADDF-C560505B88F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C022381-F1CB-4B95-AFF3-5AAF08316D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
   <si>
     <t>English</t>
   </si>
@@ -231,6 +231,12 @@
   </si>
   <si>
     <t xml:space="preserve">NHẬP MẬT KHẨU CỦA BẠN: </t>
+  </si>
+  <si>
+    <t>LANG</t>
+  </si>
+  <si>
+    <t>Tiếng Việt</t>
   </si>
 </sst>
 </file>
@@ -582,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EC3056-192F-4854-A94A-9A349BECDA04}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -608,232 +614,243 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
         <v>42</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>24</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Multiple Language Button
</commit_message>
<xml_diff>
--- a/languages.xlsx
+++ b/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C022381-F1CB-4B95-AFF3-5AAF08316D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53E8DB5-A24D-412B-8B5B-03C39E514821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
   <si>
     <t>English</t>
   </si>
@@ -44,36 +44,6 @@
     <t>Vietnamese</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Create</t>
-  </si>
-  <si>
-    <t>Đăng nhập</t>
-  </si>
-  <si>
-    <t>Tạo</t>
-  </si>
-  <si>
-    <t>BG-Title</t>
-  </si>
-  <si>
-    <t>BG-Title-VN</t>
-  </si>
-  <si>
-    <t>BG-Play</t>
-  </si>
-  <si>
-    <t>BG-Minigame</t>
-  </si>
-  <si>
-    <t>BG-Play-VN</t>
-  </si>
-  <si>
-    <t>BG-Minigame-VN</t>
-  </si>
-  <si>
     <t>Next</t>
   </si>
   <si>
@@ -125,9 +95,6 @@
     <t>PLAYER</t>
   </si>
   <si>
-    <t>BG-MINIGAME</t>
-  </si>
-  <si>
     <t>NEXT</t>
   </si>
   <si>
@@ -143,9 +110,6 @@
     <t>BG-TITLE</t>
   </si>
   <si>
-    <t>BG-PLAY</t>
-  </si>
-  <si>
     <t>ENTERYOURNAME</t>
   </si>
   <si>
@@ -237,6 +201,39 @@
   </si>
   <si>
     <t>Tiếng Việt</t>
+  </si>
+  <si>
+    <t>BTN-Play.png</t>
+  </si>
+  <si>
+    <t>BTN-PLAY</t>
+  </si>
+  <si>
+    <t>BTN-Play-VN.png</t>
+  </si>
+  <si>
+    <t>BTN-Minigame.png</t>
+  </si>
+  <si>
+    <t>BTN-MINIGAME</t>
+  </si>
+  <si>
+    <t>BG-Title.png</t>
+  </si>
+  <si>
+    <t>BG-Title-VN.png</t>
+  </si>
+  <si>
+    <t>BG-Create_account-VN.png</t>
+  </si>
+  <si>
+    <t>BG-Create_account.png</t>
+  </si>
+  <si>
+    <t>BG-Login-VN.png</t>
+  </si>
+  <si>
+    <t>BG-Login.png</t>
   </si>
 </sst>
 </file>
@@ -591,7 +588,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -603,7 +600,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -614,244 +611,244 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
         <v>52</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add shop to buy items
</commit_message>
<xml_diff>
--- a/languages.xlsx
+++ b/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53E8DB5-A24D-412B-8B5B-03C39E514821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E866727-B5EA-483A-B3A0-9D63F0E2EAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
   <si>
     <t>English</t>
   </si>
@@ -53,12 +53,6 @@
     <t>TIME</t>
   </si>
   <si>
-    <t>ENTER YOUR PASSWORD</t>
-  </si>
-  <si>
-    <t>ENTER YOUR EMAIL</t>
-  </si>
-  <si>
     <t>CHỤP ẢNH</t>
   </si>
   <si>
@@ -119,9 +113,6 @@
     <t>USERANDPASSWORD</t>
   </si>
   <si>
-    <t>ENTER YOUR NAME</t>
-  </si>
-  <si>
     <t>COLLECTEDCOIN</t>
   </si>
   <si>
@@ -234,6 +225,51 @@
   </si>
   <si>
     <t>BG-Login.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENTER YOUR NAME: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENTER YOUR EMAIL: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENTER YOUR PASSWORD: </t>
+  </si>
+  <si>
+    <t>STORE</t>
+  </si>
+  <si>
+    <t>BTN-Shop-VN.png</t>
+  </si>
+  <si>
+    <t>BTN-Shop.png</t>
+  </si>
+  <si>
+    <t>ITEM-1</t>
+  </si>
+  <si>
+    <t>ITEM-1.png</t>
+  </si>
+  <si>
+    <t>ITEM-2.png</t>
+  </si>
+  <si>
+    <t>ITEM-2</t>
+  </si>
+  <si>
+    <t>BUYED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đã mua: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUYED: </t>
+  </si>
+  <si>
+    <t>ITEM-3</t>
+  </si>
+  <si>
+    <t>ITEM-3.png</t>
   </si>
 </sst>
 </file>
@@ -585,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EC3056-192F-4854-A94A-9A349BECDA04}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -600,7 +636,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -611,90 +647,90 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -702,26 +738,26 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
@@ -732,123 +768,178 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
         <v>43</v>
-      </c>
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
         <v>9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
         <v>10</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
         <v>13</v>
-      </c>
-      <c r="C22" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
         <v>14</v>
       </c>
-      <c r="C23" t="s">
-        <v>16</v>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update main game && Capture result
</commit_message>
<xml_diff>
--- a/languages.xlsx
+++ b/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E866727-B5EA-483A-B3A0-9D63F0E2EAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3CDE01-1521-4CE7-8D11-D1E068152984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="81">
   <si>
     <t>English</t>
   </si>
@@ -270,6 +270,15 @@
   </si>
   <si>
     <t>ITEM-3.png</t>
+  </si>
+  <si>
+    <t>WIN</t>
+  </si>
+  <si>
+    <t>CONGRADUALATION! YOU WIN!!!</t>
+  </si>
+  <si>
+    <t>CHÚC MỪNG BẠN ĐÃ CHIẾN THẮNG</t>
   </si>
 </sst>
 </file>
@@ -621,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EC3056-192F-4854-A94A-9A349BECDA04}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -942,6 +951,17 @@
         <v>74</v>
       </c>
     </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Shift Objects y axis +75 in main game && Random y axis mystery boxs
</commit_message>
<xml_diff>
--- a/languages.xlsx
+++ b/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B8DE16-5E17-4B44-87C6-AD134DE2AE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415F7C64-F1F2-482E-9706-E1874452C548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
   <si>
     <t>English</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>BẠN ĐÃ THUA</t>
+  </si>
+  <si>
+    <t>BTN-Minigame-VN.png</t>
   </si>
 </sst>
 </file>
@@ -638,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EC3056-192F-4854-A94A-9A349BECDA04}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -745,7 +748,7 @@
         <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Add pre game scence to set coin and character's sets && Change screen mode && Center-aligned boxes in game
</commit_message>
<xml_diff>
--- a/languages.xlsx
+++ b/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415F7C64-F1F2-482E-9706-E1874452C548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD6B5AC-CE7C-4926-8762-78D25829B6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
   <si>
     <t>English</t>
   </si>
@@ -288,6 +288,15 @@
   </si>
   <si>
     <t>BTN-Minigame-VN.png</t>
+  </si>
+  <si>
+    <t>BETCOIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INPUT YOUR BET COIN: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NHẬP SỐ TIỀN BẠN MUỐN CƯỢC: </t>
   </si>
 </sst>
 </file>
@@ -639,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EC3056-192F-4854-A94A-9A349BECDA04}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -982,6 +991,17 @@
         <v>82</v>
       </c>
     </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Resolved duplicate variable name && Changed pos of exit button
</commit_message>
<xml_diff>
--- a/languages.xlsx
+++ b/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD6B5AC-CE7C-4926-8762-78D25829B6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B33E0B-A6F1-402B-AAE1-D32E6F5016C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
   </bookViews>
@@ -257,15 +257,9 @@
     <t>ITEM-2</t>
   </si>
   <si>
-    <t>BUYED</t>
-  </si>
-  <si>
     <t xml:space="preserve">Đã mua: </t>
   </si>
   <si>
-    <t xml:space="preserve">BUYED: </t>
-  </si>
-  <si>
     <t>ITEM-3</t>
   </si>
   <si>
@@ -297,6 +291,12 @@
   </si>
   <si>
     <t xml:space="preserve">NHẬP SỐ TIỀN BẠN MUỐN CƯỢC: </t>
+  </si>
+  <si>
+    <t>BOUGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOUGHT: </t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -757,7 +757,7 @@
         <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -949,57 +949,57 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" t="s">
         <v>73</v>
-      </c>
-      <c r="B28" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" t="s">
         <v>78</v>
-      </c>
-      <c r="B29" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" t="s">
         <v>84</v>
-      </c>
-      <c r="B31" t="s">
-        <v>85</v>
-      </c>
-      <c r="C31" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More sprites and adjusting boxes' spawn position
</commit_message>
<xml_diff>
--- a/languages.xlsx
+++ b/languages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\VSCode\PYGAME\GK-Gambling-Game-N9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B2BB2B-CAD7-4885-9569-74C74B56FF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70973706-A788-4A26-A6B7-B6ED88099D35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
+    <workbookView xWindow="4248" yWindow="1392" windowWidth="17280" windowHeight="8964" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -257,9 +246,6 @@
     <t>ITEM-2</t>
   </si>
   <si>
-    <t xml:space="preserve">Đã mua: </t>
-  </si>
-  <si>
     <t>ITEM-3</t>
   </si>
   <si>
@@ -284,19 +270,22 @@
     <t>BETCOIN</t>
   </si>
   <si>
-    <t xml:space="preserve">INPUT YOUR BET COIN: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NHẬP SỐ TIỀN BẠN MUỐN CƯỢC: </t>
-  </si>
-  <si>
     <t>BOUGHT</t>
   </si>
   <si>
     <t xml:space="preserve">BOUGHT: </t>
   </si>
   <si>
-    <t>CONGRATUALATIONS! YOU WIN!!!</t>
+    <t xml:space="preserve">ĐÃ MUA: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTER YOUR STAKE: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NHẬP SỐ TIỀN CƯỢC: </t>
+  </si>
+  <si>
+    <t>CONGRATULATIONS! YOU WIN!!!</t>
   </si>
 </sst>
 </file>
@@ -650,18 +639,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EC3056-192F-4854-A94A-9A349BECDA04}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.59765625" customWidth="1"/>
-    <col min="2" max="2" width="51.73046875" customWidth="1"/>
-    <col min="3" max="3" width="62.796875" customWidth="1"/>
+    <col min="1" max="1" width="31.5546875" customWidth="1"/>
+    <col min="2" max="2" width="51.77734375" customWidth="1"/>
+    <col min="3" max="3" width="62.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -672,7 +661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -683,7 +672,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -694,7 +683,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -705,7 +694,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -716,7 +705,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -727,7 +716,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -738,7 +727,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -749,7 +738,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -757,10 +746,10 @@
         <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -771,7 +760,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -782,7 +771,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -793,7 +782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -804,7 +793,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -815,7 +804,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -826,7 +815,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -837,7 +826,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -848,7 +837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -859,7 +848,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -870,7 +859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -881,7 +870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -892,7 +881,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -903,7 +892,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -914,7 +903,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -925,7 +914,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -936,7 +925,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -947,59 +936,59 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
         <v>74</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>75</v>
-      </c>
-      <c r="C27" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>76</v>
       </c>
       <c r="B29" t="s">
         <v>86</v>
       </c>
       <c r="C29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" t="s">
         <v>78</v>
       </c>
-      <c r="B30" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update coins-limit && List items && Login before play
</commit_message>
<xml_diff>
--- a/languages.xlsx
+++ b/languages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\VSCode\PYGAME\GK-Gambling-Game-N9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70973706-A788-4A26-A6B7-B6ED88099D35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C7EAD0-239D-4969-9B26-D689F9F8187B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4248" yWindow="1392" windowWidth="17280" windowHeight="8964" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="96">
   <si>
     <t>English</t>
   </si>
@@ -286,6 +286,33 @@
   </si>
   <si>
     <t>CONGRATULATIONS! YOU WIN!!!</t>
+  </si>
+  <si>
+    <t>MINIGAME-LIMIT</t>
+  </si>
+  <si>
+    <t>YOU CAN ONLY PLAY WHEN YOUR COIN IS UNDER 30!</t>
+  </si>
+  <si>
+    <t>BẠN CHỈ ĐƯỢC CHƠI KHI CÓ ÍT HƠN 30 COIN!</t>
+  </si>
+  <si>
+    <t>NOT-ENOUGH</t>
+  </si>
+  <si>
+    <t>NOT ENOUGH COINS</t>
+  </si>
+  <si>
+    <t>KHÔNG ĐỦ XU ĐỂ CHƠI</t>
+  </si>
+  <si>
+    <t>NOT-NULL</t>
+  </si>
+  <si>
+    <t>YOU MUST FILL YOUR STAKE!</t>
+  </si>
+  <si>
+    <t>BẠN PHẢI NHẬP SỐ TIỀN CƯỢC!</t>
   </si>
 </sst>
 </file>
@@ -637,20 +664,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EC3056-192F-4854-A94A-9A349BECDA04}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.5546875" customWidth="1"/>
-    <col min="2" max="2" width="51.77734375" customWidth="1"/>
-    <col min="3" max="3" width="62.77734375" customWidth="1"/>
+    <col min="1" max="1" width="31.53125" customWidth="1"/>
+    <col min="2" max="2" width="51.796875" customWidth="1"/>
+    <col min="3" max="3" width="62.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -661,7 +688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -672,7 +699,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -683,7 +710,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -694,7 +721,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -705,7 +732,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -716,7 +743,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -727,7 +754,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -738,7 +765,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -749,7 +776,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -760,7 +787,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -771,7 +798,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -782,7 +809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -793,7 +820,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -804,7 +831,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -815,7 +842,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -826,7 +853,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -837,7 +864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -848,7 +875,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -859,7 +886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -870,7 +897,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -881,7 +908,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -892,7 +919,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -903,7 +930,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -914,7 +941,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -925,7 +952,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -936,7 +963,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -947,7 +974,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -958,7 +985,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>75</v>
       </c>
@@ -969,7 +996,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -980,7 +1007,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>80</v>
       </c>
@@ -989,6 +1016,39 @@
       </c>
       <c r="C31" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added first chars set && Animated them
</commit_message>
<xml_diff>
--- a/languages.xlsx
+++ b/languages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1B7A98-13C8-4146-A707-FF04EAF7C279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C09990-89C4-4B80-AC8D-4084590A97CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="3472" windowWidth="16200" windowHeight="9308" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="102">
   <si>
     <t>English</t>
   </si>
@@ -255,9 +255,6 @@
     <t>WIN</t>
   </si>
   <si>
-    <t>CHÚC MỪNG BẠN ĐÃ CHIẾN THẮNG</t>
-  </si>
-  <si>
     <t>LOSE</t>
   </si>
   <si>
@@ -285,9 +282,6 @@
     <t xml:space="preserve">NHẬP SỐ TIỀN CƯỢC: </t>
   </si>
   <si>
-    <t>CONGRATULATIONS! YOU WIN!!!</t>
-  </si>
-  <si>
     <t>MINIGAME-LIMIT</t>
   </si>
   <si>
@@ -322,6 +316,21 @@
   </si>
   <si>
     <t>RULES-VN.png</t>
+  </si>
+  <si>
+    <t>END GAME!</t>
+  </si>
+  <si>
+    <t>GAME KẾT THÚC!</t>
+  </si>
+  <si>
+    <t>CHARSET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHOOSE PLAYERS SET: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHỌN SET NHÂN VẬT: </t>
   </si>
 </sst>
 </file>
@@ -673,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EC3056-192F-4854-A94A-9A349BECDA04}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -782,7 +791,7 @@
         <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -985,13 +994,13 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" t="s">
         <v>81</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>82</v>
-      </c>
-      <c r="C28" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
@@ -999,76 +1008,87 @@
         <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" t="s">
         <v>77</v>
-      </c>
-      <c r="B30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" t="s">
         <v>84</v>
-      </c>
-      <c r="C31" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" t="s">
         <v>87</v>
-      </c>
-      <c r="B32" t="s">
-        <v>88</v>
-      </c>
-      <c r="C32" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
         <v>90</v>
-      </c>
-      <c r="B33" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" t="s">
         <v>93</v>
-      </c>
-      <c r="B34" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" t="s">
         <v>96</v>
       </c>
-      <c r="B35" t="s">
-        <v>97</v>
-      </c>
-      <c r="C35" t="s">
-        <v>98</v>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added choose level buttons
</commit_message>
<xml_diff>
--- a/languages.xlsx
+++ b/languages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C09990-89C4-4B80-AC8D-4084590A97CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4B2D95-0DB0-4993-94B6-BBEF88B88350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
+    <workbookView xWindow="3195" yWindow="2348" windowWidth="16200" windowHeight="9307" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="105">
   <si>
     <t>English</t>
   </si>
@@ -331,6 +331,15 @@
   </si>
   <si>
     <t xml:space="preserve">CHỌN SET NHÂN VẬT: </t>
+  </si>
+  <si>
+    <t>LEVEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEVEL: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ĐỘ KHÓ: </t>
   </si>
 </sst>
 </file>
@@ -682,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EC3056-192F-4854-A94A-9A349BECDA04}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1091,6 +1100,17 @@
         <v>101</v>
       </c>
     </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed bug in main game
</commit_message>
<xml_diff>
--- a/languages.xlsx
+++ b/languages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4B2D95-0DB0-4993-94B6-BBEF88B88350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9721A068-2647-433C-BDFC-312BA3478F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="2348" windowWidth="16200" windowHeight="9307" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -285,12 +285,6 @@
     <t>MINIGAME-LIMIT</t>
   </si>
   <si>
-    <t>YOU CAN ONLY PLAY WHEN YOUR COIN IS UNDER 30!</t>
-  </si>
-  <si>
-    <t>BẠN CHỈ ĐƯỢC CHƠI KHI CÓ ÍT HƠN 30 COIN!</t>
-  </si>
-  <si>
     <t>NOT-ENOUGH</t>
   </si>
   <si>
@@ -340,6 +334,12 @@
   </si>
   <si>
     <t xml:space="preserve">ĐỘ KHÓ: </t>
+  </si>
+  <si>
+    <t>YOU CAN ONLY PLAY WHEN YOUR COIN IS UNDER 10!</t>
+  </si>
+  <si>
+    <t>BẠN CHỈ ĐƯỢC CHƠI KHI CÓ ÍT HƠN 10 COIN!</t>
   </si>
 </sst>
 </file>
@@ -693,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EC3056-192F-4854-A94A-9A349BECDA04}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1017,10 +1017,10 @@
         <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
@@ -1050,65 +1050,65 @@
         <v>85</v>
       </c>
       <c r="B32" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C32" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" t="s">
         <v>88</v>
-      </c>
-      <c r="B33" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
         <v>91</v>
-      </c>
-      <c r="B34" t="s">
-        <v>92</v>
-      </c>
-      <c r="C34" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" t="s">
         <v>94</v>
-      </c>
-      <c r="B35" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" t="s">
         <v>99</v>
-      </c>
-      <c r="B36" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" t="s">
         <v>102</v>
-      </c>
-      <c r="B37" t="s">
-        <v>103</v>
-      </c>
-      <c r="C37" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Online status && Fix MANY small bug
</commit_message>
<xml_diff>
--- a/languages.xlsx
+++ b/languages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671BE670-AD71-4B85-BE29-FB4FF7D13DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7A5C02-709B-4EAB-80B0-EE2F5B284625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
+    <workbookView xWindow="3195" yWindow="2348" windowWidth="16200" windowHeight="9307" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
   <si>
     <t>English</t>
   </si>
@@ -349,6 +349,15 @@
   </si>
   <si>
     <t>MAIN-HELP-VN.png</t>
+  </si>
+  <si>
+    <t>ONLINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAYERS ONLINE: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ĐANG ONLINE: </t>
   </si>
 </sst>
 </file>
@@ -700,9 +709,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EC3056-192F-4854-A94A-9A349BECDA04}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
@@ -1131,6 +1140,17 @@
         <v>107</v>
       </c>
     </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed other bugs! Oh sh*t
</commit_message>
<xml_diff>
--- a/languages.xlsx
+++ b/languages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7A5C02-709B-4EAB-80B0-EE2F5B284625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5591E672-DA57-44DE-A798-903C91D58118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="2348" windowWidth="16200" windowHeight="9307" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{660E0F7A-1E4A-4AA6-A4FC-194AD89CD6C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="114">
   <si>
     <t>English</t>
   </si>
@@ -358,6 +358,15 @@
   </si>
   <si>
     <t xml:space="preserve">ĐANG ONLINE: </t>
+  </si>
+  <si>
+    <t>NOT-VALID</t>
+  </si>
+  <si>
+    <t>AT LEAST 10 COINS</t>
+  </si>
+  <si>
+    <t>BẠN PHẢI NHẬP ÍT NHẤT 10 XU</t>
   </si>
 </sst>
 </file>
@@ -709,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EC3056-192F-4854-A94A-9A349BECDA04}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1151,6 +1160,17 @@
         <v>110</v>
       </c>
     </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>